<commit_message>
docs: finalized excel template with all subject types
</commit_message>
<xml_diff>
--- a/public/sample_timetable_data.xlsx
+++ b/public/sample_timetable_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -534,7 +534,7 @@
         <v>YES</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -575,7 +575,7 @@
         <v>NO</v>
       </c>
       <c r="L4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -616,7 +616,7 @@
         <v>NO</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -706,25 +706,25 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>IV CSE</v>
+        <v>VI CSE</v>
       </c>
       <c r="B8" t="str">
-        <v>CS2411</v>
+        <v>CS2611</v>
       </c>
       <c r="C8" t="str">
-        <v>Theory of Computation</v>
+        <v>Cryptography and cyber security (Integrated)</v>
       </c>
       <c r="D8" t="str">
-        <v>CS</v>
+        <v>MST</v>
       </c>
       <c r="E8" t="str">
+        <v>GM</v>
+      </c>
+      <c r="F8" t="str">
+        <v>VP</v>
+      </c>
+      <c r="G8" t="str">
         <v>ND</v>
-      </c>
-      <c r="F8" t="str">
-        <v>DS</v>
-      </c>
-      <c r="G8" t="str">
-        <v>NJ</v>
       </c>
       <c r="H8" t="str">
         <v/>
@@ -742,30 +742,30 @@
         <v>4</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>IV CSE</v>
+        <v>VI CSE</v>
       </c>
       <c r="B9" t="str">
-        <v>CS2412</v>
+        <v>CS2612</v>
       </c>
       <c r="C9" t="str">
-        <v>Database Management Systems</v>
+        <v>Internet of Things (Integrated)</v>
       </c>
       <c r="D9" t="str">
-        <v>VNK</v>
+        <v>ATP</v>
       </c>
       <c r="E9" t="str">
-        <v>SSP</v>
+        <v>SSB</v>
       </c>
       <c r="F9" t="str">
-        <v>RS</v>
+        <v>CS</v>
       </c>
       <c r="G9" t="str">
-        <v>NPP</v>
+        <v>MJ</v>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -780,7 +780,7 @@
         <v>NO</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -788,22 +788,22 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>IV CSE</v>
+        <v>VI CSE</v>
       </c>
       <c r="B10" t="str">
-        <v>CS2413</v>
+        <v>EC2014</v>
       </c>
       <c r="C10" t="str">
-        <v>Computer Networks</v>
+        <v>Software Defined Networks -Open Elective - I*</v>
       </c>
       <c r="D10" t="str">
-        <v>GIM</v>
+        <v>SD1</v>
       </c>
       <c r="E10" t="str">
-        <v>LHL</v>
+        <v/>
       </c>
       <c r="F10" t="str">
-        <v>SAF</v>
+        <v>SD2</v>
       </c>
       <c r="G10" t="str">
         <v/>
@@ -812,16 +812,16 @@
         <v/>
       </c>
       <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="str">
+        <v>ECE</v>
+      </c>
+      <c r="K10" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L10">
         <v>3</v>
-      </c>
-      <c r="J10" t="str">
-        <v>CSE</v>
-      </c>
-      <c r="K10" t="str">
-        <v>NO</v>
-      </c>
-      <c r="L10">
-        <v>4</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -832,40 +832,40 @@
         <v>VI CSE</v>
       </c>
       <c r="B11" t="str">
-        <v>CS2611</v>
+        <v>ME2011</v>
       </c>
       <c r="C11" t="str">
-        <v>Cryptography and Cyber Security</v>
+        <v>Renewable Energy Technologies -Open Elective - I*</v>
       </c>
       <c r="D11" t="str">
-        <v>MST</v>
+        <v>RET1</v>
       </c>
       <c r="E11" t="str">
-        <v>GM</v>
+        <v/>
       </c>
       <c r="F11" t="str">
-        <v>VP</v>
+        <v>RET2</v>
       </c>
       <c r="G11" t="str">
-        <v>ND</v>
+        <v/>
       </c>
       <c r="H11" t="str">
         <v/>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11" t="str">
-        <v>CSE</v>
+        <v>MECH</v>
       </c>
       <c r="K11" t="str">
         <v>NO</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -873,28 +873,28 @@
         <v>VI CSE</v>
       </c>
       <c r="B12" t="str">
-        <v>CS2612</v>
+        <v>CS2V62</v>
       </c>
       <c r="C12" t="str">
-        <v>Internet of Things</v>
+        <v>Image Processing - Professional Elective - III</v>
       </c>
       <c r="D12" t="str">
-        <v>ATP</v>
+        <v>DMDP</v>
       </c>
       <c r="E12" t="str">
-        <v>SSB</v>
+        <v>VNK</v>
       </c>
       <c r="F12" t="str">
-        <v>DS</v>
+        <v/>
       </c>
       <c r="G12" t="str">
-        <v>MJ</v>
+        <v/>
       </c>
       <c r="H12" t="str">
         <v/>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J12" t="str">
         <v>CSE</v>
@@ -903,15 +903,220 @@
         <v>NO</v>
       </c>
       <c r="L12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>VI CSE</v>
+      </c>
+      <c r="B13" t="str">
+        <v>ED2VA1</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Value added course - Entrepreneurship Development</v>
+      </c>
+      <c r="D13" t="str">
+        <v>PAC</v>
+      </c>
+      <c r="E13" t="str">
+        <v>NPP</v>
+      </c>
+      <c r="F13" t="str">
+        <v>SGR</v>
+      </c>
+      <c r="G13" t="str">
+        <v>RSA</v>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="K13" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>VI CSE</v>
+      </c>
+      <c r="B14" t="str">
+        <v>IT3412</v>
+      </c>
+      <c r="C14" t="str">
+        <v>IIT Spoken Tutorial class</v>
+      </c>
+      <c r="D14" t="str">
+        <v>LA1</v>
+      </c>
+      <c r="E14" t="str">
+        <v>LA2</v>
+      </c>
+      <c r="F14" t="str">
+        <v>LA3</v>
+      </c>
+      <c r="G14" t="str">
+        <v>LA4</v>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="str">
+        <v>IT</v>
+      </c>
+      <c r="K14" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>VI CSE</v>
+      </c>
+      <c r="B15" t="str">
+        <v>CS2611</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Cryptography and cyber security (Integrated Lab)</v>
+      </c>
+      <c r="D15" t="str">
+        <v>MST</v>
+      </c>
+      <c r="E15" t="str">
+        <v>GM</v>
+      </c>
+      <c r="F15" t="str">
+        <v>VP</v>
+      </c>
+      <c r="G15" t="str">
+        <v>ND</v>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="K15" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>VI CSE</v>
+      </c>
+      <c r="B16" t="str">
+        <v>CS2612</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Internet of Things (Integrated Lab)</v>
+      </c>
+      <c r="D16" t="str">
+        <v>ATP</v>
+      </c>
+      <c r="E16" t="str">
+        <v>SSB</v>
+      </c>
+      <c r="F16" t="str">
+        <v>CS</v>
+      </c>
+      <c r="G16" t="str">
+        <v>MJ</v>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="K16" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>VI CSE</v>
+      </c>
+      <c r="B17" t="str">
+        <v>CS2698</v>
+      </c>
+      <c r="C17" t="str">
+        <v>MiniProject</v>
+      </c>
+      <c r="D17" t="str">
+        <v>SAA</v>
+      </c>
+      <c r="E17" t="str">
+        <v>RAS</v>
+      </c>
+      <c r="F17" t="str">
+        <v>RSK</v>
+      </c>
+      <c r="G17" t="str">
+        <v>RSA</v>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="K17" t="str">
+        <v>NO</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>